<commit_message>
sửa lại chỗ header
</commit_message>
<xml_diff>
--- a/template_task.xlsx
+++ b/template_task.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pana\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DinhTai\Desktop\BC32E-Capstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9190"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="24">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -62,24 +62,6 @@
     <t>Header</t>
   </si>
   <si>
-    <t xml:space="preserve">     Logo</t>
-  </si>
-  <si>
-    <t>Dev A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Navbar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Submenu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Search form</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Login popup</t>
-  </si>
-  <si>
     <t>Carousel</t>
   </si>
   <si>
@@ -120,21 +102,6 @@
   </si>
   <si>
     <t>20/5</t>
-  </si>
-  <si>
-    <t>20/6</t>
-  </si>
-  <si>
-    <t>20/7</t>
-  </si>
-  <si>
-    <t>20/8</t>
-  </si>
-  <si>
-    <t>20/9</t>
-  </si>
-  <si>
-    <t>20/10</t>
   </si>
 </sst>
 </file>
@@ -144,7 +111,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,11 +132,6 @@
     <font>
       <sz val="9"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -390,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -413,9 +375,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="3" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -426,41 +385,19 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -469,7 +406,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -482,51 +419,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -807,26 +700,26 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J986"/>
+  <dimension ref="A1:J981"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.05" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5" customWidth="1"/>
-    <col min="2" max="4" width="7.59765625" customWidth="1"/>
-    <col min="5" max="5" width="10.19921875" customWidth="1"/>
-    <col min="6" max="6" width="7.59765625" customWidth="1"/>
-    <col min="7" max="7" width="9.19921875" customWidth="1"/>
-    <col min="8" max="8" width="7.59765625" customWidth="1"/>
-    <col min="9" max="9" width="8.69921875" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+    <col min="2" max="4" width="7.5546875" customWidth="1"/>
+    <col min="5" max="5" width="10.21875" customWidth="1"/>
+    <col min="6" max="6" width="7.5546875" customWidth="1"/>
+    <col min="7" max="7" width="9.21875" customWidth="1"/>
+    <col min="8" max="8" width="7.5546875" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" customWidth="1"/>
     <col min="10" max="10" width="33" customWidth="1"/>
-    <col min="11" max="26" width="7.59765625" customWidth="1"/>
+    <col min="11" max="26" width="7.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="25.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -858,464 +751,339 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="21.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="24">
-        <v>44810</v>
-      </c>
-      <c r="D2" s="9">
-        <v>1</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="24">
-        <v>44810</v>
-      </c>
-      <c r="H2" s="11">
-        <v>1</v>
-      </c>
-      <c r="I2" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" s="28"/>
+      <c r="B2" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="15">
+        <v>44810</v>
+      </c>
+      <c r="D2" s="8">
+        <v>1</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="9"/>
+      <c r="G2" s="15">
+        <v>44810</v>
+      </c>
+      <c r="H2" s="10">
+        <v>1</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="19"/>
     </row>
-    <row r="3" spans="1:10" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:10" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="E3" s="14" t="s">
+      <c r="B3" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="15">
+        <v>44810</v>
+      </c>
+      <c r="D3" s="8">
+        <v>1</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="G3" s="15">
+        <v>44810</v>
+      </c>
+      <c r="H3" s="10">
+        <v>1</v>
+      </c>
+      <c r="I3" s="17"/>
+      <c r="J3" s="20"/>
+    </row>
+    <row r="4" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="8">
-        <v>44179</v>
-      </c>
-      <c r="H3" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="I3" s="26"/>
-      <c r="J3" s="29"/>
+      <c r="B4" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="15">
+        <v>44810</v>
+      </c>
+      <c r="D4" s="8">
+        <v>1</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="G4" s="15">
+        <v>44810</v>
+      </c>
+      <c r="H4" s="10">
+        <v>1</v>
+      </c>
+      <c r="I4" s="17"/>
+      <c r="J4" s="20"/>
     </row>
-    <row r="4" spans="1:10" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+    <row r="5" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="10">
-        <v>43647</v>
-      </c>
-      <c r="D4" s="17">
-        <f>SUM(D5:D7)/3</f>
-        <v>0.9</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="8">
-        <v>44179</v>
-      </c>
-      <c r="H4" s="18">
-        <f>SUM(H5:H7)/3</f>
-        <v>0.9</v>
-      </c>
-      <c r="I4" s="26"/>
-      <c r="J4" s="29"/>
+      <c r="B5" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="15">
+        <v>44810</v>
+      </c>
+      <c r="D5" s="8">
+        <v>1</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="G5" s="15">
+        <v>44810</v>
+      </c>
+      <c r="H5" s="10">
+        <v>1</v>
+      </c>
+      <c r="I5" s="17"/>
+      <c r="J5" s="20"/>
     </row>
-    <row r="5" spans="1:10" ht="14.25" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+    <row r="6" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="19">
-        <v>43616</v>
-      </c>
-      <c r="D5" s="17">
-        <v>1</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="19"/>
-      <c r="G5" s="8">
-        <v>44179</v>
-      </c>
-      <c r="H5" s="18">
-        <v>1</v>
-      </c>
-      <c r="I5" s="26"/>
-      <c r="J5" s="29"/>
+      <c r="B6" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="15">
+        <v>44810</v>
+      </c>
+      <c r="D6" s="8">
+        <v>1</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="G6" s="15">
+        <v>44810</v>
+      </c>
+      <c r="H6" s="10">
+        <v>1</v>
+      </c>
+      <c r="I6" s="17"/>
+      <c r="J6" s="20"/>
     </row>
-    <row r="6" spans="1:10" ht="14.25" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+    <row r="7" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="19">
-        <v>43644</v>
-      </c>
-      <c r="D6" s="17">
-        <v>0.9</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="19"/>
-      <c r="G6" s="8">
-        <v>44179</v>
-      </c>
-      <c r="H6" s="18">
-        <v>0.9</v>
-      </c>
-      <c r="I6" s="26"/>
-      <c r="J6" s="29"/>
+      <c r="B7" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="15">
+        <v>44810</v>
+      </c>
+      <c r="D7" s="8">
+        <v>1</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="15">
+        <v>44810</v>
+      </c>
+      <c r="H7" s="10">
+        <v>1</v>
+      </c>
+      <c r="I7" s="17"/>
+      <c r="J7" s="20"/>
     </row>
-    <row r="7" spans="1:10" ht="9" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+    <row r="8" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="19">
-        <v>43647</v>
-      </c>
-      <c r="D7" s="17">
-        <v>0.8</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="19"/>
-      <c r="G7" s="8">
-        <v>44179</v>
-      </c>
-      <c r="H7" s="18">
-        <v>0.8</v>
-      </c>
-      <c r="I7" s="26"/>
-      <c r="J7" s="29"/>
-    </row>
-    <row r="8" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="24">
-        <v>44810</v>
-      </c>
-      <c r="D8" s="9">
-        <v>1</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="24">
-        <v>44810</v>
-      </c>
-      <c r="H8" s="11">
-        <v>1</v>
-      </c>
-      <c r="I8" s="26"/>
-      <c r="J8" s="29"/>
+      <c r="B8" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="15">
+        <v>44810</v>
+      </c>
+      <c r="D8" s="8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="G8" s="15">
+        <v>44810</v>
+      </c>
+      <c r="H8" s="10">
+        <v>1</v>
+      </c>
+      <c r="I8" s="17"/>
+      <c r="J8" s="20"/>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="24">
-        <v>44810</v>
-      </c>
-      <c r="D9" s="9">
-        <v>1</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="24">
-        <v>44810</v>
-      </c>
-      <c r="H9" s="11">
-        <v>1</v>
-      </c>
-      <c r="I9" s="26"/>
-      <c r="J9" s="29"/>
+      <c r="A9" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="15">
+        <v>44810</v>
+      </c>
+      <c r="D9" s="8">
+        <v>1</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="9"/>
+      <c r="G9" s="15">
+        <v>44810</v>
+      </c>
+      <c r="H9" s="10">
+        <v>1</v>
+      </c>
+      <c r="I9" s="17"/>
+      <c r="J9" s="20"/>
     </row>
     <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="24">
-        <v>44810</v>
-      </c>
-      <c r="D10" s="9">
-        <v>1</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="24">
-        <v>44810</v>
-      </c>
-      <c r="H10" s="11">
-        <v>1</v>
-      </c>
-      <c r="I10" s="26"/>
-      <c r="J10" s="29"/>
+      <c r="A10" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="15">
+        <v>44810</v>
+      </c>
+      <c r="D10" s="8">
+        <v>1</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="9"/>
+      <c r="G10" s="15">
+        <v>44810</v>
+      </c>
+      <c r="H10" s="10">
+        <v>1</v>
+      </c>
+      <c r="I10" s="17"/>
+      <c r="J10" s="20"/>
     </row>
     <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="24">
-        <v>44810</v>
-      </c>
-      <c r="D11" s="9">
-        <v>1</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="24">
-        <v>44810</v>
-      </c>
-      <c r="H11" s="11">
-        <v>1</v>
-      </c>
-      <c r="I11" s="26"/>
-      <c r="J11" s="29"/>
+      <c r="A11" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="15">
+        <v>44810</v>
+      </c>
+      <c r="D11" s="8">
+        <v>1</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="15">
+        <v>44810</v>
+      </c>
+      <c r="H11" s="10">
+        <v>1</v>
+      </c>
+      <c r="I11" s="17"/>
+      <c r="J11" s="20"/>
     </row>
     <row r="12" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="24">
-        <v>44810</v>
-      </c>
-      <c r="D12" s="9">
-        <v>1</v>
-      </c>
-      <c r="E12" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="24">
-        <v>44810</v>
-      </c>
-      <c r="H12" s="11">
-        <v>1</v>
-      </c>
-      <c r="I12" s="26"/>
-      <c r="J12" s="29"/>
+      <c r="A12" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="15">
+        <v>44810</v>
+      </c>
+      <c r="D12" s="8">
+        <v>1</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="15">
+        <v>44810</v>
+      </c>
+      <c r="H12" s="10">
+        <v>1</v>
+      </c>
+      <c r="I12" s="17"/>
+      <c r="J12" s="20"/>
     </row>
     <row r="13" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="24">
-        <v>44810</v>
-      </c>
-      <c r="D13" s="9">
-        <v>1</v>
-      </c>
-      <c r="E13" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="24">
-        <v>44810</v>
-      </c>
-      <c r="H13" s="11">
-        <v>1</v>
-      </c>
-      <c r="I13" s="26"/>
-      <c r="J13" s="29"/>
+      <c r="A13" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="15">
+        <v>44810</v>
+      </c>
+      <c r="D13" s="8">
+        <v>1</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="9"/>
+      <c r="G13" s="15">
+        <v>44810</v>
+      </c>
+      <c r="H13" s="10">
+        <v>1</v>
+      </c>
+      <c r="I13" s="18"/>
+      <c r="J13" s="21"/>
     </row>
-    <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="24">
-        <v>44810</v>
-      </c>
-      <c r="D14" s="9">
-        <v>1</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="10"/>
-      <c r="G14" s="24">
-        <v>44810</v>
-      </c>
-      <c r="H14" s="11">
-        <v>1</v>
-      </c>
-      <c r="I14" s="26"/>
-      <c r="J14" s="29"/>
-    </row>
-    <row r="15" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="24">
-        <v>44810</v>
-      </c>
-      <c r="D15" s="9">
-        <v>1</v>
-      </c>
-      <c r="E15" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="24">
-        <v>44810</v>
-      </c>
-      <c r="H15" s="11">
-        <v>1</v>
-      </c>
-      <c r="I15" s="26"/>
-      <c r="J15" s="29"/>
-    </row>
-    <row r="16" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="24">
-        <v>44810</v>
-      </c>
-      <c r="D16" s="9">
-        <v>1</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="F16" s="10"/>
-      <c r="G16" s="24">
-        <v>44810</v>
-      </c>
-      <c r="H16" s="11">
-        <v>1</v>
-      </c>
-      <c r="I16" s="26"/>
-      <c r="J16" s="29"/>
-    </row>
-    <row r="17" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="24">
-        <v>44810</v>
-      </c>
-      <c r="D17" s="9">
-        <v>1</v>
-      </c>
-      <c r="E17" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="24">
-        <v>44810</v>
-      </c>
-      <c r="H17" s="11">
-        <v>1</v>
-      </c>
-      <c r="I17" s="26"/>
-      <c r="J17" s="29"/>
-    </row>
-    <row r="18" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="24">
-        <v>44810</v>
-      </c>
-      <c r="D18" s="9">
-        <v>1</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="F18" s="10"/>
-      <c r="G18" s="24">
-        <v>44810</v>
-      </c>
-      <c r="H18" s="11">
-        <v>1</v>
-      </c>
-      <c r="I18" s="27"/>
-      <c r="J18" s="30"/>
-    </row>
-    <row r="19" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2265,42 +2033,37 @@
     <row r="979" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="980" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="981" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="982" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="983" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="I2:I18"/>
-    <mergeCell ref="J2:J18"/>
+    <mergeCell ref="I2:I13"/>
+    <mergeCell ref="J2:J13"/>
   </mergeCells>
-  <conditionalFormatting sqref="D2 D4:D18">
-    <cfRule type="cellIs" dxfId="9" priority="13" operator="greaterThan">
+  <conditionalFormatting sqref="D2:D13 H3:H9">
+    <cfRule type="cellIs" dxfId="5" priority="13" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2 H4:H14">
-    <cfRule type="cellIs" dxfId="8" priority="14" operator="greaterThan">
+  <conditionalFormatting sqref="H2">
+    <cfRule type="cellIs" dxfId="4" priority="14" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H15">
+  <conditionalFormatting sqref="H10">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H16">
+  <conditionalFormatting sqref="H11">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H18">
+  <conditionalFormatting sqref="H13">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H17">
+  <conditionalFormatting sqref="H12">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>

</xml_diff>